<commit_message>
feat - style - refactor: # Se agrega la funcionalidad relacionada a los periodos de cada habitacion ## se modifica la visual de la interfaz y se planea la proxima refactorización de la misma. ## se crean carpetas tests y docs, se armonizan los nombres de todas las carpetas, faltan los archivos
</commit_message>
<xml_diff>
--- a/Data/Extracto_Validacion.xlsx
+++ b/Data/Extracto_Validacion.xlsx
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>12</v>
@@ -558,10 +558,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -571,19 +571,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -704,12 +704,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -738,12 +738,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -772,12 +772,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -806,12 +806,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -840,12 +840,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -874,12 +874,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -908,12 +908,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -942,12 +942,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
         </is>
       </c>
     </row>
@@ -976,12 +976,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1010,12 +1010,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1044,12 +1044,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1078,12 +1078,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1112,12 +1112,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1180,12 +1180,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1214,12 +1214,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2025 - 21-12-2025)</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1282,12 +1282,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1316,12 +1316,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1350,12 +1350,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1384,12 +1384,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1418,12 +1418,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1452,12 +1452,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1486,12 +1486,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>26</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
         </is>
       </c>
     </row>
@@ -1520,12 +1520,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1554,12 +1554,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1588,12 +1588,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1622,12 +1622,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1690,12 +1690,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1724,12 +1724,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1758,12 +1758,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -1792,12 +1792,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -1826,12 +1826,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -1860,12 +1860,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -1894,12 +1894,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -1928,12 +1928,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -1962,12 +1962,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -1996,12 +1996,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -2030,12 +2030,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>23, 24, 25, 26, 27, 28, 29</t>
+          <t>29</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>hardoceado con parentesis (01-10-2025 - 31-10-2025) | hardoceado con parentesis (01-11-2025 - 26-11-2025) | hardoceado con parentesis (08-12-2025 - 21-12-2025) | hardoceado con parentesis (04-01-2026 - 31-03-2026) | hardoceado con parentesis (01-04-2026 - 30-09-2026) | hardoceado con parentesis (01-10-2026 - 26-11-2026) | hardoceado con parentesis (08-12-2026 - 23-12-2026)</t>
+          <t xml:space="preserve"> (08-12-2026 - 23-12-2026)</t>
         </is>
       </c>
     </row>
@@ -2360,7 +2360,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2445,12 +2445,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2479,12 +2479,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2513,12 +2513,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2547,12 +2547,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2581,12 +2581,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2615,12 +2615,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2649,12 +2649,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2683,12 +2683,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2717,12 +2717,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2751,12 +2751,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2819,12 +2819,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -2853,12 +2853,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026)</t>
         </is>
       </c>
     </row>
@@ -2887,12 +2887,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -2921,12 +2921,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -2955,12 +2955,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -2989,12 +2989,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3023,12 +3023,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3057,12 +3057,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3091,12 +3091,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3159,12 +3159,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3193,12 +3193,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3227,12 +3227,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>2, 3, 4, 5, 6, 7</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025) |  (12-12-2025 - 27-12-2025) |  (06-01-2026 - 28-02-2026) |  (01-04-2026 - 30-04-2026) |  (01-10-2026 - 31-10-2026) |  (12-12-2026 - 27-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3261,12 +3261,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3329,12 +3329,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3363,12 +3363,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3397,12 +3397,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3431,12 +3431,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3465,12 +3465,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3499,12 +3499,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3533,12 +3533,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3567,12 +3567,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3601,12 +3601,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3635,12 +3635,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>8, 9, 10</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (01-11-2025 - 11-12-2025) |  (01-03-2026 - 31-03-2026) |  (01-11-2026 - 11-12-2026)</t>
         </is>
       </c>
     </row>
@@ -3657,24 +3657,24 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
+          <t>sgl/dbl palace premier room (jacuzzi) w/breakfast served at restaurant</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>875</v>
+        <v>775</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3691,24 +3691,24 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad)</t>
+          <t>sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>950</v>
+        <v>875</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3725,24 +3725,24 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
+          <t>tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad)</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1062.5</v>
+        <v>950</v>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3759,24 +3759,24 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
+          <t>sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1137.5</v>
+        <v>1062.5</v>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3788,29 +3788,29 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LOUNGE &amp; LE MIRADOR SUITES</t>
+          <t>SUITES</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>sgl/dbl junior suite le mirador w/breakfast served at restaurant</t>
+          <t>tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1562.5</v>
+        <v>1137.5</v>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3827,24 +3827,24 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>sgl/dbl deluxe suite le mirador w/breakfast served atrestaurant</t>
+          <t>sgl/dbl junior suite le mirador w/breakfast served at restaurant</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1775</v>
+        <v>1562.5</v>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3856,29 +3856,29 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GRAND SUITES</t>
+          <t>LOUNGE &amp; LE MIRADOR SUITES</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>sgl/dbl/tpl diplomatic suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
+          <t>sgl/dbl deluxe suite le mirador w/breakfast served atrestaurant</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1937.5</v>
+        <v>1775</v>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3895,24 +3895,24 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>tpl/ cpl diplomatic suite w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch)</t>
+          <t>sgl/dbl/tpl diplomatic suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2012.5</v>
+        <v>1937.5</v>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3929,24 +3929,24 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>sgl/dbl governor suite w/breakfast served at restaurant</t>
+          <t>tpl/ cpl diplomatic suite w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch)</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2362.5</v>
+        <v>2012.5</v>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3963,24 +3963,24 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>sgl/dbl/tpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
+          <t>sgl/dbl governor suite w/breakfast served at restaurant</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2693.75</v>
+        <v>2362.5</v>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
+          <t>11, 12</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -3997,24 +3997,58 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>tpl/cpl diplomatic suite prestige w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch 3-12 years old) )</t>
+          <t>sgl/dbl/tpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old)</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2768.75</v>
+        <v>2693.75</v>
       </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
+        <v>86</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>11, 12</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Alvear Palace (A)</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>GRAND SUITES</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>tpl/cpl diplomatic suite prestige w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch 3-12 years old) )</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2768.75</v>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="n">
         <v>87</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Low Season (01-05-2026 - 30-09-2026) | Mid Season (01-10-2025 - 31-10-2025) | Mid Season (12-12-2025 - 27-12-2025) | Mid Season (06-01-2026 - 28-02-2026) | Mid Season (01-04-2026 - 30-04-2026) | Mid Season (01-10-2026 - 31-10-2026) | Mid Season (12-12-2026 - 27-12-2026) | High Season (01-11-2025 - 11-12-2025) | High Season (01-03-2026 - 31-03-2026) | High Season (01-11-2026 - 11-12-2026) | Festive Season (28-12-2025 - 05-01-2026) | Festive Season (28-12-2026 - 05-01-2027)</t>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>11, 12</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (28-12-2025 - 05-01-2026) |  (28-12-2026 - 05-01-2027)</t>
         </is>
       </c>
     </row>
@@ -4201,11 +4235,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad), sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
+          <t>sgl/dbl palace premier room (jacuzzi) w/breakfast served at restaurant, sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad), sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
         </is>
       </c>
     </row>
@@ -4575,10 +4609,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(Sin extras registrados)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>ADDITIONAL BED: From Suite Junior</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>66.66666666666667</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4591,7 +4627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4664,24 +4700,24 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dbl/sgl park view room w/buffet breakfast</t>
+          <t>dbl/sgl skyline view room w/bb</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>520</v>
+        <v>586.67</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 25-12-2025)</t>
         </is>
       </c>
     </row>
@@ -4698,24 +4734,24 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dbl/sgl skyline view room w/bb</t>
+          <t>dbl/sgl duplex suite w/bb</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>586.67</v>
+        <v>660</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 25-12-2025)</t>
         </is>
       </c>
     </row>
@@ -4732,24 +4768,24 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dbl/sgl duplex suite w/bb</t>
+          <t>dbl/sgl corner w/bb</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>660</v>
+        <v>753.33</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 25-12-2025)</t>
         </is>
       </c>
     </row>
@@ -4766,24 +4802,24 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dbl/sgl corner w/bb</t>
+          <t>dbl/sgl porteño suite w/bb</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>753.33</v>
+        <v>833.33</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-10-2025 - 25-12-2025)</t>
         </is>
       </c>
     </row>
@@ -4800,24 +4836,26 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dbl/sgl porteño suite w/bb</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>833.33</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>dbl/sgl park view room w/buffet breakfast</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>bar 20% com</t>
+        </is>
+      </c>
       <c r="F6" t="n">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2025 - 03-01-2026)</t>
         </is>
       </c>
     </row>
@@ -4834,7 +4872,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dbl/sgl park view room w/buffet breakfast</t>
+          <t>dbl/sgl skyline view room w/bb</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -4844,16 +4882,16 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2025 - 03-01-2026)</t>
         </is>
       </c>
     </row>
@@ -4884,12 +4922,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2025 - 03-01-2026)</t>
         </is>
       </c>
     </row>
@@ -4920,12 +4958,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2025 - 03-01-2026)</t>
         </is>
       </c>
     </row>
@@ -4956,12 +4994,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2025 - 03-01-2026)</t>
         </is>
       </c>
     </row>
@@ -4978,24 +5016,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dbl/sgl park view room w/buffet breakfast</t>
+          <t>dbl/sgl skyline view room w/bb</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>393.33</v>
+        <v>453.33</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5012,24 +5050,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>dbl/sgl skyline view room w/bb</t>
+          <t>dbl/sgl duplex suite w/bb</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>453.33</v>
+        <v>506.67</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5046,24 +5084,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dbl/sgl duplex suite w/bb</t>
+          <t>dbl/sgl corner w/bb</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>506.67</v>
+        <v>586.67</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5080,24 +5118,24 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>dbl/sgl corner w/bb</t>
+          <t>dbl/sgl porteño suite w/bb</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>586.67</v>
+        <v>653.33</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5114,24 +5152,24 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>dbl/sgl porteño suite w/bb</t>
+          <t>dbl/sgl skyline view room w/bb</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>653.33</v>
+        <v>586.67</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5148,24 +5186,24 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>dbl/sgl park view room w/buffet breakfast</t>
+          <t>dbl/sgl duplex suite w/bb</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>520</v>
+        <v>660</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5182,24 +5220,24 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dbl/sgl skyline view room w/bb</t>
+          <t>dbl/sgl corner w/bb</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>586.67</v>
+        <v>753.33</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5216,24 +5254,24 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>dbl/sgl duplex suite w/bb</t>
+          <t>dbl/sgl porteño suite w/bb</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>660</v>
+        <v>833.33</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (01-05-2026 - 30-09-2026)</t>
         </is>
       </c>
     </row>
@@ -5250,24 +5288,26 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>dbl/sgl corner w/bb</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>753.33</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>dbl/sgl park view room w/buffet breakfast</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>bar 20% com</t>
+        </is>
+      </c>
       <c r="F19" t="n">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>20</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (14-02-2026 - 17-02-2026)</t>
         </is>
       </c>
     </row>
@@ -5284,24 +5324,26 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>dbl/sgl porteño suite w/bb</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>833.33</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>dbl/sgl skyline view room w/bb</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>bar 20% com</t>
+        </is>
+      </c>
       <c r="F20" t="n">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (02-04-2026 - 05-04-2026)</t>
         </is>
       </c>
     </row>
@@ -5318,7 +5360,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>dbl/sgl park view room w/buffet breakfast</t>
+          <t>dbl/sgl duplex suite w/bb</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -5328,16 +5370,16 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2026 - 03-01-2027)</t>
         </is>
       </c>
     </row>
@@ -5354,7 +5396,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>dbl/sgl skyline view room w/bb</t>
+          <t>dbl/sgl corner w/bb</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -5364,16 +5406,16 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2026 - 03-01-2027)</t>
         </is>
       </c>
     </row>
@@ -5390,7 +5432,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>dbl/sgl duplex suite w/bb</t>
+          <t>dbl/sgl porteño suite w/bb</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -5400,52 +5442,16 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Faena Hotel Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>dbl/sgl porteño suite w/bb</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>bar 20% com</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>168</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>High Season (01-10-2025 - 25-12-2025) | New Year (26-12-2025 - 03-01-2026) | Low Season (01-05-2026 - 30-09-2026) | High Season (06-01-2026 - 13-02-2026) | High Season (18-02-2026 - 01-04-2026) | High Season (06-04-2026 - 30-04-2026) | High Season (01-10-2026 - 25-12-2026) | Carnival (14-02-2026 - 17-02-2026) | Easter (02-04-2026 - 05-04-2026) | New Year (26-12-2026 - 03-01-2027)</t>
+          <t xml:space="preserve"> (26-12-2026 - 03-01-2027)</t>
         </is>
       </c>
     </row>
@@ -5570,47 +5576,47 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>New Year</t>
+          <t>High Season</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>26-12-2025</t>
+          <t>06-01-2026</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>03-01-2026</t>
+          <t>13-02-2026</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Low Season</t>
+          <t>High Season</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01-05-2026</t>
+          <t>18-02-2026</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>30-09-2026</t>
+          <t>01-04-2026</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -5619,18 +5625,18 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>06-01-2026</t>
+          <t>06-04-2026</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13-02-2026</t>
+          <t>30-04-2026</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -5639,52 +5645,52 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>18-02-2026</t>
+          <t>01-10-2026</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>01-04-2026</t>
+          <t>25-12-2026</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>High Season</t>
+          <t>New Year</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>06-04-2026</t>
+          <t>26-12-2025</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>30-04-2026</t>
+          <t>03-01-2026</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>High Season</t>
+          <t>Low Season</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01-10-2026</t>
+          <t>01-05-2026</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>25-12-2026</t>
+          <t>30-09-2026</t>
         </is>
       </c>
     </row>
@@ -5759,7 +5765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5819,6 +5825,36 @@
         <v>262.5</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Faena Hotel Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ADDITIONAL BED (For child over 12 years old)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>111.1111111111111</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Faena Hotel Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ADDITIONAL BED (For child over 12 years old)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>111.1111111111111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>